<commit_message>
Motor control test passed.
</commit_message>
<xml_diff>
--- a/doc/Motor Control Design.xlsx
+++ b/doc/Motor Control Design.xlsx
@@ -261,7 +261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -279,52 +279,38 @@
     <xf numFmtId="48" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="17">
     <dxf>
-      <numFmt numFmtId="165" formatCode="0.000"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="16" formatCode="##0.0E+0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.000"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="16" formatCode="##0.0E+0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
         <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="16" formatCode="##0.0E+0"/>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -359,30 +345,6 @@
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
       </font>
       <numFmt numFmtId="165" formatCode="0.000"/>
       <fill>
@@ -405,6 +367,68 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="16" formatCode="##0.0E+0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="16" formatCode="##0.0E+0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.000"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.000"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.000"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.000"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
@@ -426,45 +450,23 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+      </font>
+      <numFmt numFmtId="16" formatCode="##0.0E+0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor auto="1"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="16" formatCode="##0.0E+0"/>
       <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.000"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.000"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -490,51 +492,51 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:P5" totalsRowShown="0" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:P5" totalsRowShown="0" dataDxfId="16">
   <autoFilter ref="A1:P5"/>
   <tableColumns count="16">
-    <tableColumn id="3" name="Pulse period (s)" dataDxfId="3">
+    <tableColumn id="3" name="Pulse period (s)" dataDxfId="15">
       <calculatedColumnFormula>2*B2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Pol period (s)" dataDxfId="4">
+    <tableColumn id="1" name="Pol period (s)" dataDxfId="14">
       <calculatedColumnFormula>Tableau1[[#This Row],[Pulse period (s)]]/2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Pulse ticks" dataDxfId="10">
+    <tableColumn id="4" name="Pulse ticks" dataDxfId="13">
       <calculatedColumnFormula>A2*Constants!$B$1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Pol ticks" dataDxfId="9">
+    <tableColumn id="2" name="Pol ticks" dataDxfId="12">
       <calculatedColumnFormula>B2*Constants!$B$1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Counter compare value" dataDxfId="16">
-      <calculatedColumnFormula>MOD(D2,65535)</calculatedColumnFormula>
+    <tableColumn id="5" name="Counter compare value" dataDxfId="0">
+      <calculatedColumnFormula>MOD(D2,65536)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Overflow target" dataDxfId="15">
+    <tableColumn id="6" name="Overflow target" dataDxfId="11">
       <calculatedColumnFormula>INT(D2/65535)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Pulses per sec" dataDxfId="14">
+    <tableColumn id="7" name="Pulses per sec" dataDxfId="10">
       <calculatedColumnFormula>1/A2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Steps per sec" dataDxfId="13">
+    <tableColumn id="8" name="Steps per sec" dataDxfId="9">
       <calculatedColumnFormula>G2/Constants!$B$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Rotation rate (deg/s)" dataDxfId="2">
+    <tableColumn id="9" name="Rotation rate (deg/s)" dataDxfId="8">
       <calculatedColumnFormula>H2*Constants!$B$4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="Result deg for 1 s" dataDxfId="0"/>
-    <tableColumn id="11" name="Rev per sec" dataDxfId="1">
+    <tableColumn id="18" name="Result deg for 1 s" dataDxfId="7"/>
+    <tableColumn id="11" name="Rev per sec" dataDxfId="6">
       <calculatedColumnFormula>I2/360</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="pace2ticksperpol" dataDxfId="12">
+    <tableColumn id="14" name="pace2ticksperpol" dataDxfId="5">
       <calculatedColumnFormula>Tableau1[[#This Row],[Pol ticks]]/Tableau1[[#This Row],[Pace (s/rad)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Rotation rate (rad/s)" dataDxfId="8">
+    <tableColumn id="10" name="Rotation rate (rad/s)" dataDxfId="4">
       <calculatedColumnFormula>I2*PI()/180</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Pace (s/rad)" dataDxfId="7">
+    <tableColumn id="13" name="Pace (s/rad)" dataDxfId="3">
       <calculatedColumnFormula>1/Tableau1[[#This Row],[Rotation rate (rad/s)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="T std dev" dataDxfId="5"/>
-    <tableColumn id="16" name="Jitter (%)" dataDxfId="6">
+    <tableColumn id="15" name="T std dev" dataDxfId="2"/>
+    <tableColumn id="16" name="Jitter (%)" dataDxfId="1">
       <calculatedColumnFormula>Tableau1[[#This Row],[T std dev]]/Tableau1[[#This Row],[Pulse period (s)]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -808,7 +810,7 @@
   <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,8 +898,8 @@
         <f>B2*Constants!$B$1</f>
         <v>956.12800000000004</v>
       </c>
-      <c r="E2" s="7">
-        <f>MOD(D2,65535)</f>
+      <c r="E2" s="17">
+        <f t="shared" ref="E2:E5" si="0">MOD(D2,65536)</f>
         <v>956.12800000000004</v>
       </c>
       <c r="F2" s="7">
@@ -960,8 +962,8 @@
         <v>69824</v>
       </c>
       <c r="E3" s="7">
-        <f>MOD(D3,65535)</f>
-        <v>4289</v>
+        <f t="shared" si="0"/>
+        <v>4288</v>
       </c>
       <c r="F3" s="7">
         <f>INT(D3/65535)</f>
@@ -1023,8 +1025,8 @@
         <v>122736</v>
       </c>
       <c r="E4" s="7">
-        <f>MOD(D4,65535)</f>
-        <v>57201</v>
+        <f t="shared" si="0"/>
+        <v>57200</v>
       </c>
       <c r="F4" s="7">
         <f>INT(D4/65535)</f>
@@ -1086,8 +1088,8 @@
         <v>490936</v>
       </c>
       <c r="E5" s="7">
-        <f>MOD(D5,65535)</f>
-        <v>32191</v>
+        <f t="shared" si="0"/>
+        <v>32184</v>
       </c>
       <c r="F5" s="7">
         <f>INT(D5/65535)</f>

</xml_diff>